<commit_message>
vault backup: 2024-05-31 10:06:52
</commit_message>
<xml_diff>
--- a/Models traits diseases prediction.xlsx
+++ b/Models traits diseases prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manzog2/Documents/projects/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAEB63AB-74B5-094B-8F6B-F0CE87089E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8FE092-4162-EA44-B033-A52A91573499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="2300" windowWidth="32900" windowHeight="16940" xr2:uid="{E24FD4CF-5B19-F640-95CD-0E0DBE7B4239}"/>
   </bookViews>
@@ -636,12 +636,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A15" sqref="A15"/>
+      <selection pane="topRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="53.1640625" customWidth="1"/>
     <col min="3" max="3" width="34.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
@@ -948,6 +948,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
vault backup: 2024-06-13 11:37:08
</commit_message>
<xml_diff>
--- a/Models traits diseases prediction.xlsx
+++ b/Models traits diseases prediction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manzog2/Documents/projects/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8FE092-4162-EA44-B033-A52A91573499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE7A904-E6D0-AF4E-ABD0-E391904E5C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="2300" windowWidth="32900" windowHeight="16940" xr2:uid="{E24FD4CF-5B19-F640-95CD-0E0DBE7B4239}"/>
+    <workbookView xWindow="260" yWindow="1120" windowWidth="32900" windowHeight="16940" xr2:uid="{E24FD4CF-5B19-F640-95CD-0E0DBE7B4239}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F14" sqref="F14"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>